<commit_message>
Added Doubleclick event handlers
</commit_message>
<xml_diff>
--- a/InventoryWiz/InventoryWiz/bin/Debug/documents/INVENTORY_FULL.xlsx
+++ b/InventoryWiz/InventoryWiz/bin/Debug/documents/INVENTORY_FULL.xlsx
@@ -185,7 +185,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1029"/>
+  <dimension ref="A1:F1030"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0" rightToLeft="false">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -33118,7 +33118,38 @@
         </is>
       </c>
     </row>
-    <row r="1030" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row customFormat="false" ht="13.8" hidden="false" customHeight="false" collapsed="false" outlineLevel="0" r="1030">
+      <c r="A1030" s="9" t="inlineStr">
+        <is>
+          <t>xyz123</t>
+        </is>
+      </c>
+      <c r="B1030" s="9" t="inlineStr">
+        <is>
+          <t>xyz123 set</t>
+        </is>
+      </c>
+      <c r="C1030" s="9" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+      <c r="D1030" s="9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E1030" s="9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F1030" s="9" t="inlineStr">
+        <is>
+          <t>-5</t>
+        </is>
+      </c>
+    </row>
     <row r="1031" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1032" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1033" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>